<commit_message>
Adicionando roteiro de testes 6
</commit_message>
<xml_diff>
--- a/PlanodeTestes/PlanodeTesteE5-CertVet.xlsx
+++ b/PlanodeTestes/PlanodeTesteE5-CertVet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ninax\Documents\ADS\6sem\ProjetoIntegrado2\PlanodeTestes\roteiros-teste\PlanodeTestes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB18288-B76B-4084-B75C-68F1F9B52DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18104488-7DF5-4E91-AD47-D76519DA8A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="732" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="732" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de testes" sheetId="7" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="352">
   <si>
     <t>RF</t>
   </si>
@@ -1795,6 +1795,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>, exceto o campo Estado, este deve ser mantido em branco;
@@ -2291,6 +2292,70 @@
   </si>
   <si>
     <t>RF06</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Acessar a URL de login (&lt;host&gt;:3000/login);
+2. Digitar </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>código da clínica válido</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> e </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>e-mail válido</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. Selecionar o botão "Avançar";
+3. Digitar a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>senha válida</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> e selecionar botão “Login”.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2431,6 +2496,7 @@
     <font>
       <sz val="10.5"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10.5"/>
@@ -3057,7 +3123,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
@@ -3416,6 +3482,70 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="14" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="28" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="34" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3451,23 +3581,9 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="14" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="28" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3482,57 +3598,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3804,11 +3869,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E18" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3883,7 +3948,7 @@
         <v>32</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>9</v>
+        <v>351</v>
       </c>
       <c r="F3" s="101" t="s">
         <v>171</v>
@@ -4027,12 +4092,12 @@
       <c r="I9" s="41"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="132"/>
-      <c r="C10" s="133"/>
-      <c r="D10" s="133"/>
-      <c r="E10" s="133"/>
-      <c r="F10" s="133"/>
-      <c r="G10" s="134"/>
+      <c r="B10" s="164"/>
+      <c r="C10" s="165"/>
+      <c r="D10" s="165"/>
+      <c r="E10" s="165"/>
+      <c r="F10" s="165"/>
+      <c r="G10" s="166"/>
       <c r="H10" s="40"/>
       <c r="I10" s="41"/>
     </row>
@@ -4568,7 +4633,7 @@
       <c r="H35" s="99"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="145"/>
+      <c r="A36" s="132"/>
       <c r="B36" s="99"/>
       <c r="C36" s="99"/>
       <c r="D36" s="47"/>
@@ -4581,7 +4646,7 @@
       <c r="A37" s="78" t="s">
         <v>147</v>
       </c>
-      <c r="B37" s="147" t="s">
+      <c r="B37" s="134" t="s">
         <v>350</v>
       </c>
       <c r="C37" s="109" t="s">
@@ -4602,7 +4667,7 @@
       <c r="A38" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="B38" s="147" t="s">
+      <c r="B38" s="134" t="s">
         <v>350</v>
       </c>
       <c r="C38" s="109" t="s">
@@ -4623,7 +4688,7 @@
       <c r="A39" s="78" t="s">
         <v>149</v>
       </c>
-      <c r="B39" s="147" t="s">
+      <c r="B39" s="134" t="s">
         <v>350</v>
       </c>
       <c r="C39" s="109" t="s">
@@ -4644,7 +4709,7 @@
       <c r="A40" s="78" t="s">
         <v>150</v>
       </c>
-      <c r="B40" s="147" t="s">
+      <c r="B40" s="134" t="s">
         <v>350</v>
       </c>
       <c r="C40" s="109" t="s">
@@ -4665,7 +4730,7 @@
       <c r="A41" s="78" t="s">
         <v>151</v>
       </c>
-      <c r="B41" s="147" t="s">
+      <c r="B41" s="134" t="s">
         <v>350</v>
       </c>
       <c r="C41" s="109" t="s">
@@ -4686,7 +4751,7 @@
       <c r="A42" s="78" t="s">
         <v>152</v>
       </c>
-      <c r="B42" s="148" t="s">
+      <c r="B42" s="135" t="s">
         <v>350</v>
       </c>
       <c r="C42" s="109" t="s">
@@ -4698,7 +4763,7 @@
       <c r="E42" s="110" t="s">
         <v>332</v>
       </c>
-      <c r="F42" s="179" t="s">
+      <c r="F42" s="159" t="s">
         <v>333</v>
       </c>
       <c r="G42" s="73"/>
@@ -4707,7 +4772,7 @@
       <c r="A43" s="78" t="s">
         <v>157</v>
       </c>
-      <c r="B43" s="148" t="s">
+      <c r="B43" s="135" t="s">
         <v>350</v>
       </c>
       <c r="C43" s="109" t="s">
@@ -4722,13 +4787,13 @@
       <c r="F43" s="109" t="s">
         <v>276</v>
       </c>
-      <c r="G43" s="149"/>
+      <c r="G43" s="136"/>
     </row>
     <row r="44" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="78" t="s">
         <v>189</v>
       </c>
-      <c r="B44" s="148" t="s">
+      <c r="B44" s="135" t="s">
         <v>350</v>
       </c>
       <c r="C44" s="109" t="s">
@@ -4743,13 +4808,13 @@
       <c r="F44" s="109" t="s">
         <v>279</v>
       </c>
-      <c r="G44" s="149"/>
+      <c r="G44" s="136"/>
     </row>
     <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="78" t="s">
         <v>334</v>
       </c>
-      <c r="B45" s="148" t="s">
+      <c r="B45" s="135" t="s">
         <v>350</v>
       </c>
       <c r="C45" s="109" t="s">
@@ -4764,10 +4829,10 @@
       <c r="F45" s="109" t="s">
         <v>282</v>
       </c>
-      <c r="G45" s="149"/>
+      <c r="G45" s="136"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="146"/>
+      <c r="A46" s="133"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G9" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
@@ -4825,7 +4890,7 @@
       <c r="D5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="150" t="s">
+      <c r="E5" s="137" t="s">
         <v>296</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -4841,7 +4906,7 @@
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="150" t="s">
+      <c r="C8" s="137" t="s">
         <v>249</v>
       </c>
       <c r="D8" s="57" t="s">
@@ -4849,7 +4914,7 @@
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="150" t="s">
+      <c r="C9" s="137" t="s">
         <v>250</v>
       </c>
       <c r="D9" s="57" t="s">
@@ -4857,7 +4922,7 @@
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="150" t="s">
+      <c r="C10" s="137" t="s">
         <v>251</v>
       </c>
       <c r="D10" s="57" t="s">
@@ -4865,7 +4930,7 @@
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="150" t="s">
+      <c r="C11" s="137" t="s">
         <v>252</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -4873,7 +4938,7 @@
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="150" t="s">
+      <c r="C12" s="137" t="s">
         <v>253</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -4881,7 +4946,7 @@
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="150" t="s">
+      <c r="C13" s="137" t="s">
         <v>254</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -4889,7 +4954,7 @@
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="150" t="s">
+      <c r="C14" s="137" t="s">
         <v>308</v>
       </c>
       <c r="D14" s="57" t="s">
@@ -4897,7 +4962,7 @@
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="150" t="s">
+      <c r="C15" s="137" t="s">
         <v>309</v>
       </c>
       <c r="D15" s="57" t="s">
@@ -4905,10 +4970,10 @@
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="150" t="s">
+      <c r="D17" s="137" t="s">
         <v>297</v>
       </c>
-      <c r="E17" s="150" t="s">
+      <c r="E17" s="137" t="s">
         <v>298</v>
       </c>
       <c r="F17" s="57" t="s">
@@ -4924,7 +4989,7 @@
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C20" s="150" t="s">
+      <c r="C20" s="137" t="s">
         <v>299</v>
       </c>
       <c r="D20" s="57" t="s">
@@ -4932,7 +4997,7 @@
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C21" s="150" t="s">
+      <c r="C21" s="137" t="s">
         <v>300</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -4940,7 +5005,7 @@
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="150" t="s">
+      <c r="C22" s="137" t="s">
         <v>301</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -4948,7 +5013,7 @@
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C23" s="150" t="s">
+      <c r="C23" s="137" t="s">
         <v>302</v>
       </c>
       <c r="D23" s="57" t="s">
@@ -4956,7 +5021,7 @@
       </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C24" s="150" t="s">
+      <c r="C24" s="137" t="s">
         <v>303</v>
       </c>
       <c r="D24" s="57" t="s">
@@ -4964,7 +5029,7 @@
       </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C25" s="150" t="s">
+      <c r="C25" s="137" t="s">
         <v>304</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -4972,7 +5037,7 @@
       </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C26" s="150" t="s">
+      <c r="C26" s="137" t="s">
         <v>305</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -4980,7 +5045,7 @@
       </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C27" s="150" t="s">
+      <c r="C27" s="137" t="s">
         <v>306</v>
       </c>
       <c r="D27" s="57" t="s">
@@ -4988,7 +5053,7 @@
       </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C28" s="150" t="s">
+      <c r="C28" s="137" t="s">
         <v>307</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -4997,10 +5062,10 @@
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C31" s="84"/>
-      <c r="D31" s="150" t="s">
+      <c r="D31" s="137" t="s">
         <v>310</v>
       </c>
-      <c r="E31" s="150" t="s">
+      <c r="E31" s="137" t="s">
         <v>311</v>
       </c>
       <c r="F31" s="84" t="s">
@@ -5016,7 +5081,7 @@
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="150" t="s">
+      <c r="C34" s="137" t="s">
         <v>312</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -5024,7 +5089,7 @@
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="150" t="s">
+      <c r="C35" s="137" t="s">
         <v>313</v>
       </c>
       <c r="D35" s="84" t="s">
@@ -5032,7 +5097,7 @@
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" s="150" t="s">
+      <c r="C36" s="137" t="s">
         <v>314</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -5040,7 +5105,7 @@
       </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C37" s="150" t="s">
+      <c r="C37" s="137" t="s">
         <v>315</v>
       </c>
       <c r="D37" s="84" t="s">
@@ -5048,7 +5113,7 @@
       </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C38" s="150" t="s">
+      <c r="C38" s="137" t="s">
         <v>316</v>
       </c>
       <c r="D38" s="84" t="s">
@@ -5056,7 +5121,7 @@
       </c>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C39" s="150" t="s">
+      <c r="C39" s="137" t="s">
         <v>317</v>
       </c>
       <c r="D39" s="84" t="s">
@@ -5064,7 +5129,7 @@
       </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C40" s="150" t="s">
+      <c r="C40" s="137" t="s">
         <v>318</v>
       </c>
       <c r="D40" s="87" t="s">
@@ -5072,7 +5137,7 @@
       </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C41" s="150" t="s">
+      <c r="C41" s="137" t="s">
         <v>319</v>
       </c>
       <c r="D41" s="87" t="s">
@@ -5080,10 +5145,10 @@
       </c>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D43" s="150" t="s">
+      <c r="D43" s="137" t="s">
         <v>320</v>
       </c>
-      <c r="E43" s="150" t="s">
+      <c r="E43" s="137" t="s">
         <v>294</v>
       </c>
       <c r="F43" s="127" t="s">
@@ -5099,7 +5164,7 @@
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C46" s="150" t="s">
+      <c r="C46" s="137" t="s">
         <v>33</v>
       </c>
       <c r="D46" s="127" t="s">
@@ -5107,7 +5172,7 @@
       </c>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C47" s="150" t="s">
+      <c r="C47" s="137" t="s">
         <v>43</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -5115,7 +5180,7 @@
       </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C48" s="150" t="s">
+      <c r="C48" s="137" t="s">
         <v>44</v>
       </c>
       <c r="D48" s="127" t="s">
@@ -5123,7 +5188,7 @@
       </c>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C49" s="150" t="s">
+      <c r="C49" s="137" t="s">
         <v>45</v>
       </c>
       <c r="D49" s="127" t="s">
@@ -5131,7 +5196,7 @@
       </c>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C50" s="150" t="s">
+      <c r="C50" s="137" t="s">
         <v>46</v>
       </c>
       <c r="D50" s="127" t="s">
@@ -5139,7 +5204,7 @@
       </c>
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C51" s="150" t="s">
+      <c r="C51" s="137" t="s">
         <v>30</v>
       </c>
       <c r="D51" s="127" t="s">
@@ -5147,29 +5212,29 @@
       </c>
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D53" s="150" t="s">
+      <c r="D53" s="137" t="s">
         <v>320</v>
       </c>
-      <c r="E53" s="150" t="s">
+      <c r="E53" s="137" t="s">
         <v>295</v>
       </c>
-      <c r="F53" s="150" t="s">
+      <c r="F53" s="137" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C54" s="150"/>
+      <c r="C54" s="137"/>
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C55" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D55" s="150" t="s">
+      <c r="D55" s="137" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C56" s="150" t="s">
+      <c r="C56" s="137" t="s">
         <v>147</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -5177,15 +5242,15 @@
       </c>
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="150" t="s">
+      <c r="C57" s="137" t="s">
         <v>148</v>
       </c>
-      <c r="D57" s="150" t="s">
+      <c r="D57" s="137" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="58" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C58" s="150" t="s">
+      <c r="C58" s="137" t="s">
         <v>149</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -5193,39 +5258,39 @@
       </c>
     </row>
     <row r="59" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C59" s="150" t="s">
+      <c r="C59" s="137" t="s">
         <v>150</v>
       </c>
-      <c r="D59" s="150" t="s">
+      <c r="D59" s="137" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C60" s="150" t="s">
+      <c r="C60" s="137" t="s">
         <v>151</v>
       </c>
-      <c r="D60" s="150" t="s">
+      <c r="D60" s="137" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C61" s="150" t="s">
+      <c r="C61" s="137" t="s">
         <v>152</v>
       </c>
-      <c r="D61" s="150" t="s">
+      <c r="D61" s="137" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="62" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="150" t="s">
+      <c r="C62" s="137" t="s">
         <v>157</v>
       </c>
-      <c r="D62" s="150" t="s">
+      <c r="D62" s="137" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="63" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C63" s="150" t="s">
+      <c r="C63" s="137" t="s">
         <v>189</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -5233,10 +5298,10 @@
       </c>
     </row>
     <row r="64" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C64" s="150" t="s">
+      <c r="C64" s="137" t="s">
         <v>334</v>
       </c>
-      <c r="D64" s="150" t="s">
+      <c r="D64" s="137" t="s">
         <v>280</v>
       </c>
     </row>
@@ -5325,10 +5390,10 @@
       <c r="D4" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="173" t="s">
+      <c r="E4" s="153" t="s">
         <v>210</v>
       </c>
-      <c r="F4" s="173" t="s">
+      <c r="F4" s="153" t="s">
         <v>283</v>
       </c>
       <c r="G4" s="3"/>
@@ -5345,10 +5410,10 @@
       <c r="A5" s="54"/>
       <c r="B5" s="44"/>
       <c r="C5" s="56"/>
-      <c r="D5" s="173" t="s">
+      <c r="D5" s="153" t="s">
         <v>335</v>
       </c>
-      <c r="E5" s="173" t="s">
+      <c r="E5" s="153" t="s">
         <v>336</v>
       </c>
       <c r="F5" s="44"/>
@@ -5370,7 +5435,7 @@
       <c r="E6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="176" t="s">
+      <c r="F6" s="156" t="s">
         <v>337</v>
       </c>
       <c r="G6" s="2"/>
@@ -5381,7 +5446,7 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="54" t="s">
         <v>62</v>
       </c>
@@ -5412,67 +5477,67 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="135" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="167" t="s">
         <v>350</v>
       </c>
-      <c r="B8" s="136" t="s">
+      <c r="B8" s="168" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="177" t="s">
+      <c r="D8" s="157" t="s">
         <v>326</v>
       </c>
-      <c r="E8" s="177" t="s">
+      <c r="E8" s="157" t="s">
         <v>342</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="136"/>
+      <c r="H8" s="168"/>
       <c r="I8" s="43"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="135"/>
-      <c r="B9" s="137"/>
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="167"/>
+      <c r="B9" s="169"/>
       <c r="C9" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="174" t="s">
+      <c r="D9" s="154" t="s">
         <v>338</v>
       </c>
-      <c r="E9" s="174" t="s">
+      <c r="E9" s="154" t="s">
         <v>343</v>
       </c>
       <c r="F9" s="48"/>
       <c r="G9" s="17"/>
-      <c r="H9" s="137"/>
+      <c r="H9" s="169"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="135"/>
-      <c r="B10" s="138"/>
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="167"/>
+      <c r="B10" s="170"/>
       <c r="C10" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="178" t="s">
+      <c r="D10" s="158" t="s">
         <v>339</v>
       </c>
-      <c r="E10" s="178" t="s">
+      <c r="E10" s="158" t="s">
         <v>344</v>
       </c>
       <c r="F10" s="49"/>
       <c r="G10" s="20"/>
-      <c r="H10" s="138"/>
+      <c r="H10" s="170"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -5480,20 +5545,20 @@
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="135"/>
-      <c r="B11" s="138"/>
-      <c r="C11" s="180" t="s">
+      <c r="A11" s="167"/>
+      <c r="B11" s="170"/>
+      <c r="C11" s="160" t="s">
         <v>106</v>
       </c>
-      <c r="D11" s="178" t="s">
+      <c r="D11" s="158" t="s">
         <v>341</v>
       </c>
-      <c r="E11" s="178" t="s">
+      <c r="E11" s="158" t="s">
         <v>345</v>
       </c>
       <c r="F11" s="49"/>
       <c r="G11" s="20"/>
-      <c r="H11" s="138"/>
+      <c r="H11" s="170"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -5501,29 +5566,29 @@
       <c r="M11" s="2"/>
     </row>
     <row r="12" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="135"/>
-      <c r="B12" s="138"/>
-      <c r="C12" s="180" t="s">
+      <c r="A12" s="167"/>
+      <c r="B12" s="170"/>
+      <c r="C12" s="160" t="s">
         <v>107</v>
       </c>
-      <c r="D12" s="178" t="s">
+      <c r="D12" s="158" t="s">
         <v>340</v>
       </c>
-      <c r="E12" s="178" t="s">
+      <c r="E12" s="158" t="s">
         <v>347</v>
       </c>
       <c r="F12" s="49"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="138"/>
+      <c r="H12" s="170"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="54"/>
-      <c r="B13" s="139" t="s">
+      <c r="B13" s="171" t="s">
         <v>79</v>
       </c>
       <c r="C13" s="66" t="s">
@@ -5532,12 +5597,12 @@
       <c r="D13" s="112" t="s">
         <v>235</v>
       </c>
-      <c r="E13" s="177" t="s">
+      <c r="E13" s="157" t="s">
         <v>342</v>
       </c>
       <c r="F13" s="50"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="141"/>
+      <c r="H13" s="173"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -5545,43 +5610,43 @@
       <c r="M13" s="2"/>
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="183" t="s">
+      <c r="A14" s="163" t="s">
         <v>350</v>
       </c>
-      <c r="B14" s="140"/>
+      <c r="B14" s="172"/>
       <c r="C14" s="67" t="s">
         <v>83</v>
       </c>
       <c r="D14" s="126" t="s">
         <v>236</v>
       </c>
-      <c r="E14" s="181" t="s">
+      <c r="E14" s="161" t="s">
         <v>343</v>
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="27"/>
-      <c r="H14" s="142"/>
+      <c r="H14" s="174"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="54"/>
-      <c r="B15" s="140"/>
+      <c r="B15" s="172"/>
       <c r="C15" s="67" t="s">
         <v>120</v>
       </c>
       <c r="D15" s="126" t="s">
         <v>237</v>
       </c>
-      <c r="E15" s="181" t="s">
+      <c r="E15" s="161" t="s">
         <v>344</v>
       </c>
       <c r="F15" s="51"/>
       <c r="G15" s="27"/>
-      <c r="H15" s="142"/>
+      <c r="H15" s="174"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -5590,40 +5655,40 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="54"/>
-      <c r="B16" s="140"/>
-      <c r="C16" s="182" t="s">
+      <c r="B16" s="172"/>
+      <c r="C16" s="162" t="s">
         <v>121</v>
       </c>
-      <c r="D16" s="181" t="s">
+      <c r="D16" s="161" t="s">
         <v>341</v>
       </c>
-      <c r="E16" s="181" t="s">
+      <c r="E16" s="161" t="s">
         <v>345</v>
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="27"/>
-      <c r="H16" s="142"/>
+      <c r="H16" s="174"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="54"/>
-      <c r="B17" s="140"/>
-      <c r="C17" s="182" t="s">
+      <c r="B17" s="172"/>
+      <c r="C17" s="162" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="181" t="s">
+      <c r="D17" s="161" t="s">
         <v>349</v>
       </c>
-      <c r="E17" s="181" t="s">
+      <c r="E17" s="161" t="s">
         <v>348</v>
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="27"/>
-      <c r="H17" s="142"/>
+      <c r="H17" s="174"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -5946,7 +6011,7 @@
       <c r="D4" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="173" t="s">
+      <c r="E4" s="153" t="s">
         <v>321</v>
       </c>
       <c r="F4" s="116" t="s">
@@ -5966,7 +6031,7 @@
       <c r="A5" s="54"/>
       <c r="B5" s="44"/>
       <c r="C5" s="56"/>
-      <c r="D5" s="173" t="s">
+      <c r="D5" s="153" t="s">
         <v>57</v>
       </c>
       <c r="E5" s="116" t="s">
@@ -6034,10 +6099,10 @@
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="135" t="s">
+      <c r="A8" s="167" t="s">
         <v>255</v>
       </c>
-      <c r="B8" s="136" t="s">
+      <c r="B8" s="168" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -6051,7 +6116,7 @@
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="136"/>
+      <c r="H8" s="168"/>
       <c r="I8" s="43"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -6059,8 +6124,8 @@
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="135"/>
-      <c r="B9" s="137"/>
+      <c r="A9" s="167"/>
+      <c r="B9" s="169"/>
       <c r="C9" s="48" t="s">
         <v>73</v>
       </c>
@@ -6072,7 +6137,7 @@
       </c>
       <c r="F9" s="48"/>
       <c r="G9" s="17"/>
-      <c r="H9" s="137"/>
+      <c r="H9" s="169"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -6080,8 +6145,8 @@
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="135"/>
-      <c r="B10" s="138"/>
+      <c r="A10" s="167"/>
+      <c r="B10" s="170"/>
       <c r="C10" s="65" t="s">
         <v>76</v>
       </c>
@@ -6093,7 +6158,7 @@
       </c>
       <c r="F10" s="49"/>
       <c r="G10" s="20"/>
-      <c r="H10" s="138"/>
+      <c r="H10" s="170"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -6101,8 +6166,8 @@
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="135"/>
-      <c r="B11" s="138"/>
+      <c r="A11" s="167"/>
+      <c r="B11" s="170"/>
       <c r="C11" s="83" t="s">
         <v>106</v>
       </c>
@@ -6114,7 +6179,7 @@
       </c>
       <c r="F11" s="49"/>
       <c r="G11" s="20"/>
-      <c r="H11" s="138"/>
+      <c r="H11" s="170"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -6123,7 +6188,7 @@
     </row>
     <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="54"/>
-      <c r="B12" s="139" t="s">
+      <c r="B12" s="171" t="s">
         <v>79</v>
       </c>
       <c r="C12" s="66" t="s">
@@ -6137,7 +6202,7 @@
       </c>
       <c r="F12" s="50"/>
       <c r="G12" s="13"/>
-      <c r="H12" s="141"/>
+      <c r="H12" s="173"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -6148,7 +6213,7 @@
       <c r="A13" s="131" t="s">
         <v>255</v>
       </c>
-      <c r="B13" s="140"/>
+      <c r="B13" s="172"/>
       <c r="C13" s="67" t="s">
         <v>83</v>
       </c>
@@ -6160,7 +6225,7 @@
       </c>
       <c r="F13" s="51"/>
       <c r="G13" s="27"/>
-      <c r="H13" s="142"/>
+      <c r="H13" s="174"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -6169,7 +6234,7 @@
     </row>
     <row r="14" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="54"/>
-      <c r="B14" s="140"/>
+      <c r="B14" s="172"/>
       <c r="C14" s="67" t="s">
         <v>120</v>
       </c>
@@ -6181,7 +6246,7 @@
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="27"/>
-      <c r="H14" s="142"/>
+      <c r="H14" s="174"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -6190,7 +6255,7 @@
     </row>
     <row r="15" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="54"/>
-      <c r="B15" s="140"/>
+      <c r="B15" s="172"/>
       <c r="C15" s="91" t="s">
         <v>121</v>
       </c>
@@ -6202,7 +6267,7 @@
       </c>
       <c r="F15" s="51"/>
       <c r="G15" s="27"/>
-      <c r="H15" s="142"/>
+      <c r="H15" s="174"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -6525,7 +6590,7 @@
       <c r="D4" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="173" t="s">
+      <c r="E4" s="153" t="s">
         <v>322</v>
       </c>
       <c r="F4" s="81" t="s">
@@ -6545,7 +6610,7 @@
       <c r="A5" s="54"/>
       <c r="B5" s="44"/>
       <c r="C5" s="56"/>
-      <c r="D5" s="173" t="s">
+      <c r="D5" s="153" t="s">
         <v>323</v>
       </c>
       <c r="E5" s="85" t="s">
@@ -6613,10 +6678,10 @@
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="135" t="s">
+      <c r="A8" s="167" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="136" t="s">
+      <c r="B8" s="168" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -6630,7 +6695,7 @@
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="136"/>
+      <c r="H8" s="168"/>
       <c r="I8" s="43"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -6638,12 +6703,12 @@
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="135"/>
-      <c r="B9" s="137"/>
+      <c r="A9" s="167"/>
+      <c r="B9" s="169"/>
       <c r="C9" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="174" t="s">
+      <c r="D9" s="154" t="s">
         <v>224</v>
       </c>
       <c r="E9" s="89" t="s">
@@ -6651,7 +6716,7 @@
       </c>
       <c r="F9" s="48"/>
       <c r="G9" s="17"/>
-      <c r="H9" s="137"/>
+      <c r="H9" s="169"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -6659,8 +6724,8 @@
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="135"/>
-      <c r="B10" s="138"/>
+      <c r="A10" s="167"/>
+      <c r="B10" s="170"/>
       <c r="C10" s="65" t="s">
         <v>76</v>
       </c>
@@ -6672,7 +6737,7 @@
       </c>
       <c r="F10" s="49"/>
       <c r="G10" s="20"/>
-      <c r="H10" s="138"/>
+      <c r="H10" s="170"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -6680,8 +6745,8 @@
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="135"/>
-      <c r="B11" s="138"/>
+      <c r="A11" s="167"/>
+      <c r="B11" s="170"/>
       <c r="C11" s="83" t="s">
         <v>106</v>
       </c>
@@ -6693,7 +6758,7 @@
       </c>
       <c r="F11" s="49"/>
       <c r="G11" s="20"/>
-      <c r="H11" s="138"/>
+      <c r="H11" s="170"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -6701,8 +6766,8 @@
       <c r="M11" s="2"/>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="135"/>
-      <c r="B12" s="138"/>
+      <c r="A12" s="167"/>
+      <c r="B12" s="170"/>
       <c r="C12" s="83" t="s">
         <v>107</v>
       </c>
@@ -6714,7 +6779,7 @@
       </c>
       <c r="F12" s="49"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="138"/>
+      <c r="H12" s="170"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -6722,8 +6787,8 @@
       <c r="M12" s="2"/>
     </row>
     <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="135"/>
-      <c r="B13" s="138"/>
+      <c r="A13" s="167"/>
+      <c r="B13" s="170"/>
       <c r="C13" s="83" t="s">
         <v>155</v>
       </c>
@@ -6735,7 +6800,7 @@
       </c>
       <c r="F13" s="49"/>
       <c r="G13" s="20"/>
-      <c r="H13" s="138"/>
+      <c r="H13" s="170"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -6743,8 +6808,8 @@
       <c r="M13" s="2"/>
     </row>
     <row r="14" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="135"/>
-      <c r="B14" s="138"/>
+      <c r="A14" s="167"/>
+      <c r="B14" s="170"/>
       <c r="C14" s="95" t="s">
         <v>156</v>
       </c>
@@ -6756,7 +6821,7 @@
       </c>
       <c r="F14" s="49"/>
       <c r="G14" s="20"/>
-      <c r="H14" s="138"/>
+      <c r="H14" s="170"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -6765,7 +6830,7 @@
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="54"/>
-      <c r="B15" s="139" t="s">
+      <c r="B15" s="171" t="s">
         <v>79</v>
       </c>
       <c r="C15" s="66" t="s">
@@ -6779,7 +6844,7 @@
       </c>
       <c r="F15" s="50"/>
       <c r="G15" s="13"/>
-      <c r="H15" s="141"/>
+      <c r="H15" s="173"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -6790,7 +6855,7 @@
       <c r="A16" s="96" t="s">
         <v>144</v>
       </c>
-      <c r="B16" s="140"/>
+      <c r="B16" s="172"/>
       <c r="C16" s="67" t="s">
         <v>83</v>
       </c>
@@ -6802,7 +6867,7 @@
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="27"/>
-      <c r="H16" s="142"/>
+      <c r="H16" s="174"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -6811,7 +6876,7 @@
     </row>
     <row r="17" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="54"/>
-      <c r="B17" s="140"/>
+      <c r="B17" s="172"/>
       <c r="C17" s="67" t="s">
         <v>120</v>
       </c>
@@ -6823,7 +6888,7 @@
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="27"/>
-      <c r="H17" s="142"/>
+      <c r="H17" s="174"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -6832,7 +6897,7 @@
     </row>
     <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="54"/>
-      <c r="B18" s="140"/>
+      <c r="B18" s="172"/>
       <c r="C18" s="91" t="s">
         <v>121</v>
       </c>
@@ -6844,7 +6909,7 @@
       </c>
       <c r="F18" s="51"/>
       <c r="G18" s="27"/>
-      <c r="H18" s="142"/>
+      <c r="H18" s="174"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -6853,7 +6918,7 @@
     </row>
     <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="54"/>
-      <c r="B19" s="140"/>
+      <c r="B19" s="172"/>
       <c r="C19" s="91" t="s">
         <v>122</v>
       </c>
@@ -6865,7 +6930,7 @@
       </c>
       <c r="F19" s="51"/>
       <c r="G19" s="27"/>
-      <c r="H19" s="142"/>
+      <c r="H19" s="174"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -6874,7 +6939,7 @@
     </row>
     <row r="20" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="54"/>
-      <c r="B20" s="140"/>
+      <c r="B20" s="172"/>
       <c r="C20" s="91" t="s">
         <v>190</v>
       </c>
@@ -6886,7 +6951,7 @@
       </c>
       <c r="F20" s="51"/>
       <c r="G20" s="27"/>
-      <c r="H20" s="142"/>
+      <c r="H20" s="174"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -6897,7 +6962,7 @@
     </row>
     <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="54"/>
-      <c r="B21" s="140"/>
+      <c r="B21" s="172"/>
       <c r="C21" s="91" t="s">
         <v>191</v>
       </c>
@@ -6909,7 +6974,7 @@
       </c>
       <c r="F21" s="51"/>
       <c r="G21" s="27"/>
-      <c r="H21" s="142"/>
+      <c r="H21" s="174"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -6918,7 +6983,7 @@
     </row>
     <row r="22" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="54"/>
-      <c r="B22" s="143"/>
+      <c r="B22" s="175"/>
       <c r="C22" s="92" t="s">
         <v>199</v>
       </c>
@@ -6930,7 +6995,7 @@
       </c>
       <c r="F22" s="52"/>
       <c r="G22" s="32"/>
-      <c r="H22" s="144"/>
+      <c r="H22" s="176"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -7179,7 +7244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -7253,7 +7318,7 @@
       <c r="D4" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="173" t="s">
+      <c r="E4" s="153" t="s">
         <v>324</v>
       </c>
       <c r="F4" s="58" t="s">
@@ -7273,7 +7338,7 @@
       <c r="A5" s="54"/>
       <c r="B5" s="44"/>
       <c r="C5" s="56"/>
-      <c r="D5" s="173" t="s">
+      <c r="D5" s="153" t="s">
         <v>325</v>
       </c>
       <c r="E5" s="58" t="s">
@@ -7341,10 +7406,10 @@
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="135" t="s">
+      <c r="A8" s="167" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="136" t="s">
+      <c r="B8" s="168" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -7358,7 +7423,7 @@
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="136"/>
+      <c r="H8" s="168"/>
       <c r="I8" s="43"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -7366,8 +7431,8 @@
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="135"/>
-      <c r="B9" s="137"/>
+      <c r="A9" s="167"/>
+      <c r="B9" s="169"/>
       <c r="C9" s="48" t="s">
         <v>73</v>
       </c>
@@ -7379,7 +7444,7 @@
       </c>
       <c r="F9" s="48"/>
       <c r="G9" s="17"/>
-      <c r="H9" s="137"/>
+      <c r="H9" s="169"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -7387,8 +7452,8 @@
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="135"/>
-      <c r="B10" s="138"/>
+      <c r="A10" s="167"/>
+      <c r="B10" s="170"/>
       <c r="C10" s="65" t="s">
         <v>76</v>
       </c>
@@ -7400,7 +7465,7 @@
       </c>
       <c r="F10" s="49"/>
       <c r="G10" s="20"/>
-      <c r="H10" s="138"/>
+      <c r="H10" s="170"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -7408,8 +7473,8 @@
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A11" s="135"/>
-      <c r="B11" s="138"/>
+      <c r="A11" s="167"/>
+      <c r="B11" s="170"/>
       <c r="C11" s="65" t="s">
         <v>106</v>
       </c>
@@ -7421,7 +7486,7 @@
       </c>
       <c r="F11" s="49"/>
       <c r="G11" s="20"/>
-      <c r="H11" s="138"/>
+      <c r="H11" s="170"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -7429,8 +7494,8 @@
       <c r="M11" s="2"/>
     </row>
     <row r="12" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="135"/>
-      <c r="B12" s="138"/>
+      <c r="A12" s="167"/>
+      <c r="B12" s="170"/>
       <c r="C12" s="65" t="s">
         <v>107</v>
       </c>
@@ -7442,7 +7507,7 @@
       </c>
       <c r="F12" s="49"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="138"/>
+      <c r="H12" s="170"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -7451,7 +7516,7 @@
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="54"/>
-      <c r="B13" s="139" t="s">
+      <c r="B13" s="171" t="s">
         <v>79</v>
       </c>
       <c r="C13" s="66" t="s">
@@ -7465,7 +7530,7 @@
       </c>
       <c r="F13" s="50"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="141"/>
+      <c r="H13" s="173"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -7474,7 +7539,7 @@
     </row>
     <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="54"/>
-      <c r="B14" s="140"/>
+      <c r="B14" s="172"/>
       <c r="C14" s="67" t="s">
         <v>83</v>
       </c>
@@ -7486,7 +7551,7 @@
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="27"/>
-      <c r="H14" s="142"/>
+      <c r="H14" s="174"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -7495,7 +7560,7 @@
     </row>
     <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="54"/>
-      <c r="B15" s="140"/>
+      <c r="B15" s="172"/>
       <c r="C15" s="67" t="s">
         <v>120</v>
       </c>
@@ -7507,7 +7572,7 @@
       </c>
       <c r="F15" s="51"/>
       <c r="G15" s="27"/>
-      <c r="H15" s="142"/>
+      <c r="H15" s="174"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -7516,7 +7581,7 @@
     </row>
     <row r="16" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="54"/>
-      <c r="B16" s="140"/>
+      <c r="B16" s="172"/>
       <c r="C16" s="67" t="s">
         <v>121</v>
       </c>
@@ -7528,7 +7593,7 @@
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="27"/>
-      <c r="H16" s="142"/>
+      <c r="H16" s="174"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -7539,7 +7604,7 @@
     </row>
     <row r="17" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="54"/>
-      <c r="B17" s="143"/>
+      <c r="B17" s="175"/>
       <c r="C17" s="69" t="s">
         <v>122</v>
       </c>
@@ -7551,7 +7616,7 @@
       </c>
       <c r="F17" s="52"/>
       <c r="G17" s="32"/>
-      <c r="H17" s="144"/>
+      <c r="H17" s="176"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -7856,7 +7921,7 @@
       <c r="D4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="175" t="s">
+      <c r="E4" s="155" t="s">
         <v>296</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -7874,7 +7939,7 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="175" t="s">
+      <c r="D5" s="155" t="s">
         <v>261</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -7927,10 +7992,10 @@
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="135" t="s">
+      <c r="A8" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="136" t="s">
+      <c r="B8" s="168" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -7944,11 +8009,11 @@
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="136"/>
+      <c r="H8" s="168"/>
     </row>
     <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="135"/>
-      <c r="B9" s="137"/>
+      <c r="A9" s="167"/>
+      <c r="B9" s="169"/>
       <c r="C9" s="14" t="s">
         <v>73</v>
       </c>
@@ -7960,11 +8025,11 @@
       </c>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
-      <c r="H9" s="137"/>
+      <c r="H9" s="169"/>
     </row>
     <row r="10" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="135"/>
-      <c r="B10" s="138"/>
+      <c r="A10" s="167"/>
+      <c r="B10" s="170"/>
       <c r="C10" s="18" t="s">
         <v>76</v>
       </c>
@@ -7976,10 +8041,10 @@
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
-      <c r="H10" s="138"/>
+      <c r="H10" s="170"/>
     </row>
     <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="139" t="s">
+      <c r="B11" s="171" t="s">
         <v>79</v>
       </c>
       <c r="C11" s="21" t="s">
@@ -7993,10 +8058,10 @@
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="13"/>
-      <c r="H11" s="141"/>
+      <c r="H11" s="173"/>
     </row>
     <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="140"/>
+      <c r="B12" s="172"/>
       <c r="C12" s="23"/>
       <c r="D12" s="24" t="s">
         <v>82</v>
@@ -8006,13 +8071,13 @@
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="27"/>
-      <c r="H12" s="142"/>
+      <c r="H12" s="174"/>
       <c r="L12" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="143"/>
+      <c r="B13" s="175"/>
       <c r="C13" s="28" t="s">
         <v>83</v>
       </c>
@@ -8024,7 +8089,7 @@
       </c>
       <c r="F13" s="31"/>
       <c r="G13" s="32"/>
-      <c r="H13" s="144"/>
+      <c r="H13" s="176"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D14" s="33" t="s">
@@ -8098,39 +8163,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51" style="171" customWidth="1"/>
-    <col min="2" max="2" width="69.42578125" style="171" customWidth="1"/>
+    <col min="1" max="1" width="51" style="151" customWidth="1"/>
+    <col min="2" max="2" width="69.42578125" style="151" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="170" t="s">
+      <c r="A1" s="177" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="170"/>
+      <c r="A2" s="177"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="171" t="s">
+      <c r="A3" s="151" t="s">
         <v>288</v>
       </c>
-      <c r="B3" s="171" t="s">
+      <c r="B3" s="151" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="171" t="s">
+      <c r="A4" s="151" t="s">
         <v>290</v>
       </c>
-      <c r="B4" s="171" t="s">
+      <c r="B4" s="151" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="172" t="s">
+      <c r="A5" s="152" t="s">
         <v>292</v>
       </c>
-      <c r="B5" s="172" t="s">
+      <c r="B5" s="152" t="s">
         <v>293</v>
       </c>
     </row>
@@ -8159,98 +8224,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="181" t="s">
         <v>286</v>
       </c>
-      <c r="B1" s="158"/>
+      <c r="B1" s="182"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="140" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="160" t="s">
+      <c r="B2" s="141" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="142" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="162">
+      <c r="B3" s="143">
         <v>123456</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="163"/>
-      <c r="B4" s="164"/>
+      <c r="A4" s="144"/>
+      <c r="B4" s="145"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="157" t="s">
+      <c r="A6" s="181" t="s">
         <v>285</v>
       </c>
-      <c r="B6" s="158"/>
+      <c r="B6" s="182"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="159" t="s">
+      <c r="A7" s="140" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="160" t="s">
+      <c r="B7" s="141" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="165" t="s">
+      <c r="A8" s="146" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="162" t="s">
+      <c r="B8" s="143" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="166"/>
-      <c r="B9" s="167"/>
+      <c r="A9" s="147"/>
+      <c r="B9" s="148"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="168"/>
-      <c r="B10" s="169"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11" s="153"/>
+      <c r="A10" s="149"/>
+      <c r="B10" s="150"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="154" t="s">
+      <c r="A13" s="178" t="s">
         <v>284</v>
       </c>
-      <c r="B13" s="155"/>
-      <c r="C13" s="156"/>
+      <c r="B13" s="179"/>
+      <c r="C13" s="180"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="152" t="s">
+      <c r="A14" s="139" t="s">
         <v>158</v>
       </c>
-      <c r="B14" s="151" t="s">
+      <c r="B14" s="138" t="s">
         <v>159</v>
       </c>
-      <c r="C14" s="151" t="s">
+      <c r="C14" s="138" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="151"/>
-      <c r="B15" s="151"/>
-      <c r="C15" s="151"/>
+      <c r="A15" s="138"/>
+      <c r="B15" s="138"/>
+      <c r="C15" s="138"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="151"/>
-      <c r="B16" s="151"/>
-      <c r="C16" s="151"/>
+      <c r="A16" s="138"/>
+      <c r="B16" s="138"/>
+      <c r="C16" s="138"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="151"/>
-      <c r="B17" s="151"/>
-      <c r="C17" s="151"/>
+      <c r="A17" s="138"/>
+      <c r="B17" s="138"/>
+      <c r="C17" s="138"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>